<commit_message>
made all parameters dynamic , code to format txt data without headers
</commit_message>
<xml_diff>
--- a/stock_predictor/Timesheet.xlsx
+++ b/stock_predictor/Timesheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prgs\Code\mokshtech\stock_predictor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prgs\Code\mokshtech1\stock_predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
   <si>
     <t>Mon</t>
   </si>
@@ -197,6 +197,60 @@
   </si>
   <si>
     <t>report analyss, rnn model flag implementaion, dela date data fetch implementation , drop duplicate rows implemetation, drop na rows implementation</t>
+  </si>
+  <si>
+    <t>meeting , dynamic base path.</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> future date inreporting</t>
+  </si>
+  <si>
+    <t>direct run from cmd line, directly forcast without predictions</t>
+  </si>
+  <si>
+    <t>1+2</t>
+  </si>
+  <si>
+    <t>2+2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forcast directly for a new symbol, model for 5 min data </t>
+  </si>
+  <si>
+    <t>svr</t>
+  </si>
+  <si>
+    <t>rf</t>
+  </si>
+  <si>
+    <t>testing and ensambing</t>
+  </si>
+  <si>
+    <t>ensambling + meeting</t>
+  </si>
+  <si>
+    <t>code to format minute data text file,  testing with minutes data, ensambling</t>
+  </si>
+  <si>
+    <t>make all parametersdynamic and testing,ensambling</t>
   </si>
 </sst>
 </file>
@@ -212,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -331,6 +391,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -620,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:C34"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,10 +700,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12">
+      <c r="A1" s="14">
         <v>43191</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
@@ -653,7 +717,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>35</v>
       </c>
@@ -671,7 +735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -709,7 +773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -727,7 +791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -745,7 +809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -757,7 +821,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -769,7 +833,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -787,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -805,7 +869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -825,7 +889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -837,7 +901,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -849,7 +913,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -861,7 +925,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -873,7 +937,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -891,7 +955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -929,7 +993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -947,7 +1011,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -965,7 +1029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -985,7 +1049,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
@@ -997,7 +1061,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -1009,7 +1073,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
@@ -1045,7 +1109,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -1063,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
@@ -1079,7 +1143,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -1112,7 +1176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1132,7 +1196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1152,7 +1216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
@@ -1172,14 +1236,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="1">
         <v>2</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="15" t="s">
         <v>52</v>
       </c>
       <c r="D33" s="2"/>
@@ -1190,14 +1254,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B34" s="1">
         <v>3</v>
       </c>
-      <c r="C34" s="14"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="2"/>
       <c r="E34" s="1">
         <v>4</v>
@@ -1213,24 +1277,308 @@
       <c r="B35" s="1">
         <v>4</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="1"/>
+      <c r="C35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="1">
+        <v>3</v>
+      </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="1">
+        <v>9</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="2">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="1">
+        <v>10</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="1">
+        <v>3</v>
+      </c>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="1">
+        <v>11</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="1">
+        <v>3</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="1">
+        <v>12</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="2">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1">
+        <v>4</v>
+      </c>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="1">
+        <v>13</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="2">
+        <v>4</v>
+      </c>
+      <c r="E41" s="1">
+        <v>4</v>
+      </c>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="1">
         <v>14</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1">
-        <f>SUM(E2:E35)</f>
-        <v>77</v>
-      </c>
-      <c r="F36" s="1">
-        <f>SUM(F2:F35)</f>
+      <c r="C42" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="2">
+        <v>4</v>
+      </c>
+      <c r="E42" s="1">
+        <v>4</v>
+      </c>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="1">
+        <v>15</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="2">
+        <v>4</v>
+      </c>
+      <c r="E43" s="1">
+        <v>4</v>
+      </c>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="1">
+        <v>16</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E44" s="1">
+        <v>4</v>
+      </c>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" s="1">
+        <v>17</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="1">
+        <v>18</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="1">
+        <v>3</v>
+      </c>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="1">
+        <v>19</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="1">
+        <v>20</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="1">
+        <v>21</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" s="1">
+        <v>4</v>
+      </c>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="1">
+        <v>22</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="1">
+        <v>23</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1">
+        <f>SUM(E2:E54)</f>
+        <v>120</v>
+      </c>
+      <c r="F55" s="1">
+        <f>SUM(F2:F54)</f>
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix reporting for nifty,added model name in report
</commit_message>
<xml_diff>
--- a/stock_predictor/Timesheet.xlsx
+++ b/stock_predictor/Timesheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prgs\Code\mokshtech1\stock_predictor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Prgs\Code\mokshtech\stock_predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -391,10 +391,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,6 +400,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,10 +700,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14">
+      <c r="A1" s="12">
         <v>43191</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="B33" s="1">
         <v>2</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="13" t="s">
         <v>52</v>
       </c>
       <c r="D33" s="2"/>
@@ -1261,7 +1261,7 @@
       <c r="B34" s="1">
         <v>3</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="14"/>
       <c r="D34" s="2"/>
       <c r="E34" s="1">
         <v>4</v>
@@ -1483,9 +1483,9 @@
       <c r="B47" s="1">
         <v>19</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="13"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="16"/>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1495,9 +1495,9 @@
       <c r="B48" s="1">
         <v>20</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="13"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="16"/>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1525,9 +1525,9 @@
       <c r="B50" s="1">
         <v>22</v>
       </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="13"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="16"/>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,9 +1537,9 @@
       <c r="B51" s="1">
         <v>23</v>
       </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="13"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="16"/>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
dateprecesion,forcast value precesion setting
</commit_message>
<xml_diff>
--- a/stock_predictor/Timesheet.xlsx
+++ b/stock_predictor/Timesheet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="73">
   <si>
     <t>Mon</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>make all parametersdynamic and testing,ensambling</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Nifty Fix, modelname in report , formating forcast values to 2 decimal and formating timestamp to minutes</t>
   </si>
 </sst>
 </file>
@@ -374,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -391,6 +397,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,10 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,15 +702,15 @@
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="1.5703125" customWidth="1"/>
+    <col min="6" max="6" width="0.42578125" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="14">
         <v>43191</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="14"/>
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
@@ -716,8 +723,11 @@
       <c r="F1" s="11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>35</v>
       </c>
@@ -735,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -753,7 +763,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -773,7 +783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -791,7 +801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -809,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -821,7 +831,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -833,7 +843,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -851,7 +861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -889,7 +899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -901,7 +911,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>3</v>
       </c>
@@ -913,7 +923,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -925,7 +935,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -937,7 +947,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>6</v>
       </c>
@@ -1243,7 +1253,7 @@
       <c r="B33" s="1">
         <v>2</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="15" t="s">
         <v>52</v>
       </c>
       <c r="D33" s="2"/>
@@ -1261,7 +1271,7 @@
       <c r="B34" s="1">
         <v>3</v>
       </c>
-      <c r="C34" s="14"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="2"/>
       <c r="E34" s="1">
         <v>4</v>
@@ -1286,7 +1296,9 @@
       <c r="E35" s="1">
         <v>3</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
@@ -1312,7 +1324,9 @@
       <c r="E37" s="1">
         <v>3</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1330,7 +1344,9 @@
       <c r="E38" s="1">
         <v>3</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -1348,7 +1364,9 @@
       <c r="E39" s="1">
         <v>3</v>
       </c>
-      <c r="F39" s="1"/>
+      <c r="F39" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -1366,7 +1384,9 @@
       <c r="E40" s="1">
         <v>4</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1384,7 +1404,9 @@
       <c r="E41" s="1">
         <v>4</v>
       </c>
-      <c r="F41" s="1"/>
+      <c r="F41" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -1402,7 +1424,9 @@
       <c r="E42" s="1">
         <v>4</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -1420,7 +1444,9 @@
       <c r="E43" s="1">
         <v>4</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -1438,7 +1464,9 @@
       <c r="E44" s="1">
         <v>4</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -1456,7 +1484,9 @@
       <c r="E45" s="1">
         <v>4</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -1474,7 +1504,9 @@
       <c r="E46" s="1">
         <v>3</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -1483,9 +1515,9 @@
       <c r="B47" s="1">
         <v>19</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="16"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="13"/>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1495,9 +1527,9 @@
       <c r="B48" s="1">
         <v>20</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="16"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13"/>
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1516,7 +1548,9 @@
       <c r="E49" s="1">
         <v>4</v>
       </c>
-      <c r="F49" s="1"/>
+      <c r="F49" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
@@ -1525,9 +1559,9 @@
       <c r="B50" s="1">
         <v>22</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="16"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="13"/>
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1537,49 +1571,193 @@
       <c r="B51" s="1">
         <v>23</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="16"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="13"/>
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="1">
+        <v>24</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="1">
+        <v>25</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F53" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="1">
+        <v>26</v>
+      </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="1">
+        <v>27</v>
+      </c>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="1">
+        <v>28</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="1">
+        <v>29</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="1">
+        <v>30</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" s="1">
+        <v>31</v>
+      </c>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60" s="17">
+        <v>1</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="17">
+        <v>2</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B62" s="17">
+        <v>3</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="17">
+        <v>4</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1">
         <f>SUM(E2:E54)</f>
-        <v>120</v>
-      </c>
-      <c r="F55" s="1">
+        <v>121.5</v>
+      </c>
+      <c r="F65" s="1">
         <f>SUM(F2:F54)</f>
-        <v>105</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change flow of options download and calucaiton
</commit_message>
<xml_diff>
--- a/stock_predictor/Timesheet.xlsx
+++ b/stock_predictor/Timesheet.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="80">
   <si>
     <t>Mon</t>
   </si>
@@ -269,6 +269,15 @@
   </si>
   <si>
     <t>Options IV</t>
+  </si>
+  <si>
+    <t>Options IV and DB</t>
+  </si>
+  <si>
+    <t>DB pushed all stock data, fetching latest date and fetch delta data</t>
+  </si>
+  <si>
+    <t>DB, upload delta data,change flow of file Options download and calcultate IV</t>
   </si>
 </sst>
 </file>
@@ -432,15 +441,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -450,6 +450,15 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,7 +743,7 @@
   <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,10 +756,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="14">
+      <c r="A1" s="20">
         <v>43191</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
@@ -1293,7 +1302,7 @@
       <c r="B33" s="1">
         <v>2</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="21" t="s">
         <v>52</v>
       </c>
       <c r="D33" s="2"/>
@@ -1311,7 +1320,7 @@
       <c r="B34" s="1">
         <v>3</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="2"/>
       <c r="E34" s="1">
         <v>4</v>
@@ -1349,19 +1358,19 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B37" s="18">
+      <c r="B37" s="15">
         <v>9</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="19">
-        <v>3</v>
-      </c>
-      <c r="E37" s="18">
+      <c r="D37" s="16">
+        <v>3</v>
+      </c>
+      <c r="E37" s="15">
         <v>3</v>
       </c>
       <c r="F37" s="1">
@@ -1688,7 +1697,7 @@
       <c r="A56" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="17">
+      <c r="B56" s="14">
         <v>43276</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -1704,7 +1713,7 @@
       <c r="A57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B57" s="17">
+      <c r="B57" s="14">
         <v>43277</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -1720,7 +1729,7 @@
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="17">
+      <c r="B58" s="14">
         <v>43278</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -1758,13 +1767,13 @@
       <c r="E60" s="13">
         <v>0</v>
       </c>
-      <c r="F60" s="20"/>
+      <c r="F60" s="17"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="21">
+      <c r="B61" s="18">
         <v>43291</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -1774,13 +1783,13 @@
       <c r="E61" s="1">
         <v>2</v>
       </c>
-      <c r="F61" s="20"/>
+      <c r="F61" s="17"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="21">
+      <c r="B62" s="18">
         <v>43292</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -1790,13 +1799,13 @@
       <c r="E62" s="1">
         <v>3</v>
       </c>
-      <c r="F62" s="20"/>
+      <c r="F62" s="17"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B63" s="21">
+      <c r="B63" s="18">
         <v>43293</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -1806,13 +1815,13 @@
       <c r="E63" s="1">
         <v>3.5</v>
       </c>
-      <c r="F63" s="20"/>
+      <c r="F63" s="17"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B64" s="21">
+      <c r="B64" s="18">
         <v>43294</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -1827,7 +1836,7 @@
       <c r="A65" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B65" s="21">
+      <c r="B65" s="18">
         <v>43295</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -1842,7 +1851,7 @@
       <c r="A66" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B66" s="21">
+      <c r="B66" s="18">
         <v>43296</v>
       </c>
       <c r="C66" s="12"/>
@@ -1855,10 +1864,10 @@
       <c r="A67" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="21">
+      <c r="B67" s="18">
         <v>43297</v>
       </c>
-      <c r="C67" s="22" t="s">
+      <c r="C67" s="19" t="s">
         <v>76</v>
       </c>
       <c r="D67" s="1"/>
@@ -1870,7 +1879,7 @@
       <c r="A68" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="21">
+      <c r="B68" s="18">
         <v>43298</v>
       </c>
       <c r="C68" s="12"/>
@@ -1883,10 +1892,10 @@
       <c r="A69" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B69" s="21">
+      <c r="B69" s="18">
         <v>43299</v>
       </c>
-      <c r="C69" s="22" t="s">
+      <c r="C69" s="19" t="s">
         <v>76</v>
       </c>
       <c r="D69" s="1"/>
@@ -1898,11 +1907,11 @@
       <c r="A70" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B70" s="21">
+      <c r="B70" s="18">
         <v>43300</v>
       </c>
-      <c r="C70" s="22" t="s">
-        <v>76</v>
+      <c r="C70" s="19" t="s">
+        <v>77</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="5">
@@ -1913,7 +1922,7 @@
       <c r="A71" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B71" s="21">
+      <c r="B71" s="18">
         <v>43301</v>
       </c>
       <c r="C71" s="12"/>
@@ -1926,7 +1935,7 @@
       <c r="A72" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B72" s="21">
+      <c r="B72" s="18">
         <v>43302</v>
       </c>
       <c r="C72" s="12"/>
@@ -1939,23 +1948,31 @@
       <c r="A73" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="21">
+      <c r="B73" s="18">
         <v>43303</v>
       </c>
-      <c r="C73" s="1"/>
+      <c r="C73" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
+      <c r="E73" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B74" s="21">
+      <c r="B74" s="18">
         <v>43304</v>
       </c>
-      <c r="C74" s="1"/>
+      <c r="C74" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
+      <c r="E74" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
@@ -1973,9 +1990,9 @@
       <c r="D76" s="1"/>
       <c r="E76" s="1">
         <f>SUM(E2:E75)</f>
-        <v>156.5</v>
-      </c>
-      <c r="F76" s="20"/>
+        <v>165.5</v>
+      </c>
+      <c r="F76" s="17"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F77" s="1">

</xml_diff>